<commit_message>
add real case with 8 locations
</commit_message>
<xml_diff>
--- a/config/realword_5/RL_5_locations.xlsx
+++ b/config/realword_5/RL_5_locations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/captainzhang/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/captainzhang/Documents/Research/scheduling/Drone/Drone_route_plainning/config/realword_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7158ACE5-7913-7D47-8B0F-75F859A4417E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66230EA-63E0-9043-87AE-2B85F09605C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{2D1AB624-8524-174B-B5AF-7B1C794377DB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{2D1AB624-8524-174B-B5AF-7B1C794377DB}"/>
   </bookViews>
   <sheets>
     <sheet name="best_route" sheetId="1" r:id="rId1"/>
@@ -1053,11 +1053,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1088,8 +1088,15 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1122,7 +1129,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1187,7 +1194,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1505,17 +1512,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2361E6E5-3CDB-5446-8186-9C6FEB86C4D8}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="223" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="223" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1532,7 +1539,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1549,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1566,7 +1573,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1583,7 +1590,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1600,7 +1607,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1617,7 +1624,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1635,6 +1642,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1643,18 +1651,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32B2CD7-DC10-364A-B123-8FF61D91E302}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView zoomScale="176" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="176" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1662,7 +1668,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -1670,7 +1676,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -1678,7 +1684,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1686,7 +1692,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -1694,7 +1700,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -1702,7 +1708,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1710,617 +1716,618 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="3">
         <v>323.33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="3">
         <v>431.97</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" s="3">
         <v>375.7</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="3">
         <v>337.57</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="3">
         <v>184.22</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63" s="3">
         <v>347.33</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71" s="3">
         <v>450.97</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1">
       <c r="A77" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1">
       <c r="A79" s="3">
         <v>418.7</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1">
       <c r="A80" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1">
       <c r="A81" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1">
       <c r="A82" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1">
       <c r="A83" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1">
       <c r="A84" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1">
       <c r="A85" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1">
       <c r="A86" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1">
       <c r="A87" s="3">
         <v>370.57</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1">
       <c r="A88" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1">
       <c r="A89" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1">
       <c r="A90" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1">
       <c r="A91" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1">
       <c r="A92" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1">
       <c r="A93" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1">
       <c r="A94" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1">
       <c r="A95" s="3">
         <v>233.22</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1">
       <c r="A96" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1">
       <c r="A97" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1">
       <c r="A98" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1">
       <c r="A99" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1">
       <c r="A100" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1">
       <c r="A101" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1">
       <c r="A102" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1">
       <c r="A103" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1">
       <c r="A104" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1">
       <c r="A106" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1">
       <c r="A107" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1">
       <c r="A108" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1">
       <c r="A109" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1">
       <c r="A110" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1">
       <c r="A111" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1">
       <c r="A112" s="3">
         <v>200</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1">
       <c r="A115" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1">
       <c r="A117" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1">
       <c r="A118" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1">
       <c r="A119" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1">
       <c r="A120" s="3">
         <v>250</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1">
       <c r="A121" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1">
       <c r="A122" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1">
       <c r="A123" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1">
       <c r="A124" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1">
       <c r="A125" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1">
       <c r="A126" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1">
       <c r="A127" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1">
       <c r="A128" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130" s="1" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2331,8 +2338,9 @@
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>